<commit_message>
Rendering first style alien
</commit_message>
<xml_diff>
--- a/Nyk/assets/Alien Shapes.xlsx
+++ b/Nyk/assets/Alien Shapes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\JavaScript\Game\Nyk\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BA8FDF-6DC9-4AFC-858F-39BB3023DE36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9A436D-2BF2-430F-B179-5A5FA3337763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D95CB183-1229-4A80-848E-DFAC974CAB93}"/>
   </bookViews>
@@ -540,9 +540,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-15</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1848,7 +1845,7 @@
   <dimension ref="A2:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -2094,11 +2091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G17" s="1">
-        <f>COUNT(J4:J40)</f>
-        <v>37</v>
-      </c>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J17" s="1">
         <v>-10</v>
       </c>
@@ -2106,7 +2099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J18" s="1">
         <v>10</v>
       </c>
@@ -2114,7 +2107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J19" s="1">
         <v>10</v>
       </c>
@@ -2122,7 +2115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J20" s="1">
         <v>25</v>
       </c>
@@ -2130,7 +2123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J21" s="1">
         <v>25</v>
       </c>
@@ -2138,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J22" s="1">
         <v>30</v>
       </c>
@@ -2146,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J23" s="1">
         <v>30</v>
       </c>
@@ -2154,7 +2147,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="24" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J24" s="1">
         <v>20</v>
       </c>
@@ -2162,7 +2155,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="25" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J25" s="1">
         <v>20</v>
       </c>
@@ -2170,7 +2163,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="26" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J26" s="1">
         <v>25</v>
       </c>
@@ -2178,7 +2171,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="27" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J27" s="1">
         <v>25</v>
       </c>
@@ -2186,7 +2179,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="28" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J28" s="1">
         <v>20</v>
       </c>
@@ -2194,7 +2187,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="29" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J29" s="1">
         <v>20</v>
       </c>
@@ -2202,7 +2195,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="30" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J30" s="1">
         <v>10</v>
       </c>
@@ -2210,7 +2203,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="31" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J31" s="1">
         <v>10</v>
       </c>
@@ -2218,7 +2211,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="32" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J32" s="1">
         <v>15</v>
       </c>

</xml_diff>